<commit_message>
DONE Sequence Diagram, Class Diagram, Task Management, Database design
</commit_message>
<xml_diff>
--- a/KH_HUE_T08_DatabaseDesign_v1.0.xlsx
+++ b/KH_HUE_T08_DatabaseDesign_v1.0.xlsx
@@ -264,9 +264,8 @@
     <font>
       <sz val="18"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -685,7 +684,7 @@
   <dimension ref="B1:V120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>